<commit_message>
Added proper manager Billing corection
</commit_message>
<xml_diff>
--- a/templates/leave_data_template.xlsx
+++ b/templates/leave_data_template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>OT ID</t>
   </si>
@@ -55,64 +55,31 @@
     <t>ABC</t>
   </si>
   <si>
+    <t>V001</t>
+  </si>
+  <si>
+    <t>V002</t>
+  </si>
+  <si>
     <t>dsad</t>
   </si>
   <si>
-    <t>dsds</t>
-  </si>
-  <si>
-    <t>sds</t>
-  </si>
-  <si>
-    <t>dss</t>
-  </si>
-  <si>
-    <t>csc</t>
-  </si>
-  <si>
-    <t>sc</t>
-  </si>
-  <si>
-    <t>cx</t>
-  </si>
-  <si>
-    <t>asv</t>
-  </si>
-  <si>
-    <t>9/4/2023</t>
-  </si>
-  <si>
-    <t>9/1/2023</t>
-  </si>
-  <si>
-    <t>8/21/2023</t>
-  </si>
-  <si>
-    <t>8/14/2023</t>
-  </si>
-  <si>
-    <t>7/31/2023</t>
-  </si>
-  <si>
-    <t>7/3/2023</t>
-  </si>
-  <si>
-    <t>1/16/2024</t>
-  </si>
-  <si>
-    <t>1/9/2024</t>
-  </si>
-  <si>
-    <t>1/8/2024</t>
-  </si>
-  <si>
-    <t>1/1/2024</t>
-  </si>
-  <si>
-    <t>7/7/2023</t>
-  </si>
-  <si>
-    <t>1/12/2024</t>
+    <t>pers001</t>
+  </si>
+  <si>
+    <t>pers002</t>
+  </si>
+  <si>
+    <t>9/4/2025</t>
+  </si>
+  <si>
+    <t>9/7/2025</t>
+  </si>
+  <si>
+    <t>9/10/2025</t>
+  </si>
+  <si>
+    <t>9/12/2025</t>
   </si>
   <si>
     <t>Earned Leave(EL)</t>
@@ -128,9 +95,6 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>...</t>
   </si>
 </sst>
 </file>
@@ -488,7 +452,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -537,28 +501,28 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="G2" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="H2">
         <v>8</v>
       </c>
       <c r="I2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -566,37 +530,37 @@
       <c r="K2">
         <v>1</v>
       </c>
-      <c r="L2" t="s">
-        <v>38</v>
+      <c r="L2">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="H3">
         <v>8</v>
       </c>
       <c r="I3" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -604,312 +568,46 @@
       <c r="K3">
         <v>1</v>
       </c>
-      <c r="L3" t="s">
-        <v>38</v>
+      <c r="L3">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="H4">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="I4" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4">
         <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5">
-        <v>4</v>
-      </c>
-      <c r="I5" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5">
-        <v>0.5</v>
-      </c>
-      <c r="K5">
-        <v>0.5</v>
-      </c>
-      <c r="L5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6">
-        <v>8</v>
-      </c>
-      <c r="I6" t="s">
-        <v>37</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7">
-        <v>40</v>
-      </c>
-      <c r="I7" t="s">
-        <v>37</v>
-      </c>
-      <c r="J7">
-        <v>5</v>
-      </c>
-      <c r="K7">
-        <v>11</v>
-      </c>
-      <c r="L7">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8">
-        <v>8</v>
-      </c>
-      <c r="I8" t="s">
-        <v>37</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="L8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9">
-        <v>32</v>
-      </c>
-      <c r="I9" t="s">
-        <v>37</v>
-      </c>
-      <c r="J9">
-        <v>4</v>
-      </c>
-      <c r="K9">
-        <v>4</v>
-      </c>
-      <c r="L9">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" t="s">
-        <v>36</v>
-      </c>
-      <c r="H10">
-        <v>8</v>
-      </c>
-      <c r="I10" t="s">
-        <v>37</v>
-      </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-      <c r="L10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11">
-        <v>56</v>
-      </c>
-      <c r="I11" t="s">
-        <v>37</v>
-      </c>
-      <c r="J11">
-        <v>7</v>
-      </c>
-      <c r="K11">
-        <v>8</v>
-      </c>
-      <c r="L11">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>